<commit_message>
fix split date template
</commit_message>
<xml_diff>
--- a/comoOdeCpp/tests/testthat/data/Template_CoMoCOVID-19App_new_16.1_intv_split.xlsx
+++ b/comoOdeCpp/tests/testthat/data/Template_CoMoCOVID-19App_new_16.1_intv_split.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17850" tabRatio="871" firstSheet="3" activeTab="10"/>
+    <workbookView windowWidth="23400" windowHeight="12000" tabRatio="871" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -1786,11 +1786,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1837,10 +1837,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1851,10 +1852,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1866,9 +1875,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1883,12 +1891,35 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1896,17 +1927,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1921,52 +1951,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1982,7 +1967,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2041,37 +2041,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2083,25 +2071,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2113,37 +2083,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2161,7 +2101,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2179,43 +2209,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2318,6 +2318,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2335,9 +2359,35 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2357,56 +2407,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -2418,146 +2418,146 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2637,7 +2637,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2661,17 +2661,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3952,7 +3952,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -4120,7 +4120,7 @@
         <v>44012</v>
       </c>
       <c r="C8" s="4">
-        <v>44073</v>
+        <v>44165</v>
       </c>
       <c r="D8" s="3">
         <v>28</v>

</xml_diff>